<commit_message>
added code to present financial data as graphs, produced graphs and included in latex code and document
</commit_message>
<xml_diff>
--- a/MA_FinancialData/Datastream2/TRUS3MT.xlsx
+++ b/MA_FinancialData/Datastream2/TRUS3MT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MA_FinancialData\Datastream2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corin\Documents\Uni\M.A.HSG\MA_Arbeit\MasterThesis_NarrativesInFinance\MA_FinancialData\Datastream2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D82257-30AE-452B-885D-CA915F1E6E8F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,22 +18,27 @@
   <definedNames>
     <definedName name="TRNR_6591729c56384f90bbdf05f9dae5adb4_5218_1" hidden="1">Sheet1!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eikon, HSG</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,21 +119,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="thomsonreutersshim.dfortdformula">
-      <tp t="s">
-        <v>Name</v>
-        <stp/>
-        <stp>153170bc-74de-4b0f-a630-7bc6d4a050f7</stp>
-        <tr r="A1" s="1"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,10 +383,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5219"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5194" workbookViewId="0">
+      <selection activeCell="C5218" sqref="C5218"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -403,9 +396,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="str">
-        <f>_xll.Thomson.Reuters.AFOSpreadsheetFormulas.DSGRID("TRUS3MT"," ","1998-09-30","2018-09-30","D","RowHeader=true;ColHeader=true;DispSeriesDescription=false;YearlyTSFormat=false;QuarterlyTSFormat=false","")</f>
-        <v>Name</v>
+      <c r="A1" t="e">
+        <f ca="1">_xll.Thomson.Reuters.AFOSpreadsheetFormulas.DSGRID("TRUS3MT"," ","1998-09-30","2018-09-30","D","RowHeader=true;ColHeader=true;DispSeriesDescription=false;YearlyTSFormat=false;QuarterlyTSFormat=false","")</f>
+        <v>#NAME?</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -42155,9 +42148,17 @@
         <v>2.1989999999999998</v>
       </c>
     </row>
+    <row r="5220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5220" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B5220">
+        <v>2.206</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="TRAFO" prompt="$A$1:$B$5219" sqref="A1"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="TRAFO" prompt="$A$1:$B$5219" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>